<commit_message>
2022/10/20 10:00 basic gen
</commit_message>
<xml_diff>
--- a/programs/gen/ae_gen_pop.xlsx
+++ b/programs/gen/ae_gen_pop.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>32.32957458496094</v>
+        <v>27.66905212402344</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>32.35160064697266</v>
+        <v>27.65714645385742</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>32.30580139160156</v>
+        <v>27.6608943939209</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>32.3437614440918</v>
+        <v>27.63476943969727</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>32.31289672851562</v>
+        <v>27.5916862487793</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>32.24070739746094</v>
+        <v>27.55545997619629</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>32.24127960205078</v>
+        <v>27.55633544921875</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>32.20933532714844</v>
+        <v>27.52512741088867</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>32.14110946655273</v>
+        <v>27.48206329345703</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>31.96576690673828</v>
+        <v>27.29934310913086</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>32.11631393432617</v>
+        <v>27.40110015869141</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>32.08311080932617</v>
+        <v>27.40662002563477</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>31.74579429626465</v>
+        <v>27.42031478881836</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>31.70692253112793</v>
+        <v>27.34615325927734</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>31.76412582397461</v>
+        <v>27.42633438110352</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>31.90193557739258</v>
+        <v>27.44657516479492</v>
       </c>
     </row>
     <row r="18">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>32.03857421875</v>
+        <v>27.47085952758789</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>32.1761360168457</v>
+        <v>27.60934066772461</v>
       </c>
     </row>
     <row r="20">
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>32.07562637329102</v>
+        <v>27.59995269775391</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>32.41998291015625</v>
+        <v>27.67121124267578</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>32.44806289672852</v>
+        <v>27.67374420166016</v>
       </c>
     </row>
     <row r="23">
@@ -611,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>32.68899536132812</v>
+        <v>27.79495239257812</v>
       </c>
     </row>
     <row r="24">
@@ -619,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>32.59392929077148</v>
+        <v>27.97919464111328</v>
       </c>
     </row>
     <row r="25">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>32.63549041748047</v>
+        <v>28.11801338195801</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>32.6077880859375</v>
+        <v>28.18033218383789</v>
       </c>
     </row>
     <row r="27">
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>32.94453430175781</v>
+        <v>28.27571868896484</v>
       </c>
     </row>
     <row r="28">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>32.80158615112305</v>
+        <v>28.38410568237305</v>
       </c>
     </row>
     <row r="29">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>32.73017883300781</v>
+        <v>28.44696807861328</v>
       </c>
     </row>
     <row r="30">
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>32.46935653686523</v>
+        <v>28.4536018371582</v>
       </c>
     </row>
     <row r="31">
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>32.56793975830078</v>
+        <v>28.45384788513184</v>
       </c>
     </row>
     <row r="32">
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>32.68445587158203</v>
+        <v>28.45519828796387</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>32.44698333740234</v>
+        <v>28.4549674987793</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>32.42193603515625</v>
+        <v>28.45528602600098</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>32.33487701416016</v>
+        <v>28.44990158081055</v>
       </c>
     </row>
     <row r="36">
@@ -715,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>32.45800399780273</v>
+        <v>28.45429992675781</v>
       </c>
     </row>
     <row r="37">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>32.44301605224609</v>
+        <v>28.45492744445801</v>
       </c>
     </row>
     <row r="38">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>34.0569953918457</v>
+        <v>28.44275665283203</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>33.88664245605469</v>
+        <v>28.35370635986328</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>33.65041732788086</v>
+        <v>28.35317993164062</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>33.74748992919922</v>
+        <v>28.35382461547852</v>
       </c>
     </row>
     <row r="42">
@@ -763,7 +763,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>33.87074279785156</v>
+        <v>28.34934043884277</v>
       </c>
     </row>
     <row r="43">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>33.78415298461914</v>
+        <v>28.35287475585938</v>
       </c>
     </row>
     <row r="44">
@@ -779,7 +779,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>33.75949859619141</v>
+        <v>28.35557746887207</v>
       </c>
     </row>
     <row r="45">
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>33.77742004394531</v>
+        <v>28.35473251342773</v>
       </c>
     </row>
     <row r="46">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>33.92681884765625</v>
+        <v>28.3566780090332</v>
       </c>
     </row>
     <row r="47">
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>34.01379013061523</v>
+        <v>28.36385345458984</v>
       </c>
     </row>
     <row r="48">
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>33.92304611206055</v>
+        <v>28.35428428649902</v>
       </c>
     </row>
     <row r="49">
@@ -819,7 +819,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>33.8352165222168</v>
+        <v>28.35077285766602</v>
       </c>
     </row>
     <row r="50">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>34.28121948242188</v>
+        <v>28.49682998657227</v>
       </c>
     </row>
     <row r="51">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>34.47702789306641</v>
+        <v>28.51563262939453</v>
       </c>
     </row>
     <row r="52">
@@ -843,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>34.64385604858398</v>
+        <v>28.62179946899414</v>
       </c>
     </row>
     <row r="53">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>34.76105499267578</v>
+        <v>28.68942451477051</v>
       </c>
     </row>
     <row r="54">
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>34.91741561889648</v>
+        <v>28.71491241455078</v>
       </c>
     </row>
     <row r="55">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>34.88432693481445</v>
+        <v>28.73809623718262</v>
       </c>
     </row>
     <row r="56">
@@ -875,7 +875,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>34.62311172485352</v>
+        <v>28.7507438659668</v>
       </c>
     </row>
     <row r="57">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>34.58290481567383</v>
+        <v>28.7479190826416</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>34.48591232299805</v>
+        <v>28.71734046936035</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>34.53775024414062</v>
+        <v>28.7585506439209</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>34.68464660644531</v>
+        <v>28.76956939697266</v>
       </c>
     </row>
     <row r="61">
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>34.87088394165039</v>
+        <v>28.79003524780273</v>
       </c>
     </row>
     <row r="62">
@@ -923,7 +923,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>36.9709587097168</v>
+        <v>29.35970497131348</v>
       </c>
     </row>
     <row r="63">
@@ -931,7 +931,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>37.26652145385742</v>
+        <v>29.32793617248535</v>
       </c>
     </row>
     <row r="64">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>37.28094100952148</v>
+        <v>29.30887603759766</v>
       </c>
     </row>
     <row r="65">
@@ -947,7 +947,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>37.03621292114258</v>
+        <v>29.34774589538574</v>
       </c>
     </row>
     <row r="66">
@@ -955,7 +955,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>36.60890197753906</v>
+        <v>29.42799377441406</v>
       </c>
     </row>
     <row r="67">
@@ -963,7 +963,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>36.59679412841797</v>
+        <v>29.47896003723145</v>
       </c>
     </row>
     <row r="68">
@@ -971,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>36.15289688110352</v>
+        <v>29.64876937866211</v>
       </c>
     </row>
     <row r="69">
@@ -979,7 +979,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>36.12042617797852</v>
+        <v>29.62230682373047</v>
       </c>
     </row>
     <row r="70">
@@ -987,7 +987,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>35.7765007019043</v>
+        <v>29.65471458435059</v>
       </c>
     </row>
     <row r="71">
@@ -995,7 +995,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>36.03800964355469</v>
+        <v>29.65487670898438</v>
       </c>
     </row>
     <row r="72">
@@ -1003,7 +1003,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>36.13483047485352</v>
+        <v>29.65479278564453</v>
       </c>
     </row>
     <row r="73">
@@ -1011,7 +1011,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>36.09537506103516</v>
+        <v>29.65093803405762</v>
       </c>
     </row>
     <row r="74">
@@ -1019,7 +1019,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>35.71060943603516</v>
+        <v>29.5987377166748</v>
       </c>
     </row>
     <row r="75">
@@ -1027,7 +1027,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>35.73360443115234</v>
+        <v>29.59167098999023</v>
       </c>
     </row>
     <row r="76">
@@ -1035,7 +1035,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>35.88431549072266</v>
+        <v>29.58914947509766</v>
       </c>
     </row>
     <row r="77">
@@ -1043,7 +1043,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>35.8823356628418</v>
+        <v>29.59189987182617</v>
       </c>
     </row>
     <row r="78">
@@ -1051,7 +1051,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>35.83163833618164</v>
+        <v>29.59364700317383</v>
       </c>
     </row>
     <row r="79">
@@ -1059,7 +1059,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>35.65034103393555</v>
+        <v>29.58661651611328</v>
       </c>
     </row>
     <row r="80">
@@ -1067,7 +1067,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>35.3686637878418</v>
+        <v>29.57635688781738</v>
       </c>
     </row>
     <row r="81">
@@ -1075,7 +1075,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>35.17980194091797</v>
+        <v>29.56295394897461</v>
       </c>
     </row>
     <row r="82">
@@ -1083,7 +1083,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>34.94351959228516</v>
+        <v>29.55951309204102</v>
       </c>
     </row>
     <row r="83">
@@ -1091,7 +1091,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>35.40688323974609</v>
+        <v>29.55318069458008</v>
       </c>
     </row>
     <row r="84">
@@ -1099,7 +1099,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>35.51026153564453</v>
+        <v>29.54098701477051</v>
       </c>
     </row>
     <row r="85">
@@ -1107,7 +1107,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>35.54092788696289</v>
+        <v>29.5446720123291</v>
       </c>
     </row>
     <row r="86">
@@ -1115,7 +1115,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>35.33072280883789</v>
+        <v>29.53800010681152</v>
       </c>
     </row>
     <row r="87">
@@ -1123,7 +1123,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>35.20008850097656</v>
+        <v>29.53806495666504</v>
       </c>
     </row>
     <row r="88">
@@ -1131,7 +1131,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>35.37411117553711</v>
+        <v>29.53747177124023</v>
       </c>
     </row>
     <row r="89">
@@ -1139,7 +1139,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>35.45266342163086</v>
+        <v>29.5374927520752</v>
       </c>
     </row>
     <row r="90">
@@ -1147,7 +1147,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>35.31634902954102</v>
+        <v>29.53659057617188</v>
       </c>
     </row>
     <row r="91">
@@ -1155,7 +1155,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>35.31374740600586</v>
+        <v>29.53535842895508</v>
       </c>
     </row>
     <row r="92">
@@ -1163,7 +1163,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>35.07827377319336</v>
+        <v>29.53458786010742</v>
       </c>
     </row>
     <row r="93">
@@ -1171,7 +1171,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>35.01080703735352</v>
+        <v>29.53378295898438</v>
       </c>
     </row>
     <row r="94">
@@ -1179,7 +1179,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>34.88078689575195</v>
+        <v>29.5339412689209</v>
       </c>
     </row>
     <row r="95">
@@ -1187,7 +1187,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>34.97523498535156</v>
+        <v>29.53366088867188</v>
       </c>
     </row>
     <row r="96">
@@ -1195,7 +1195,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>35.48963165283203</v>
+        <v>29.53484153747559</v>
       </c>
     </row>
     <row r="97">
@@ -1203,7 +1203,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>35.72954940795898</v>
+        <v>29.53561782836914</v>
       </c>
     </row>
     <row r="98">
@@ -1211,7 +1211,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>35.45249176025391</v>
+        <v>29.53652572631836</v>
       </c>
     </row>
     <row r="99">
@@ -1219,7 +1219,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>34.94221496582031</v>
+        <v>29.53427124023438</v>
       </c>
     </row>
     <row r="100">
@@ -1227,7 +1227,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>35.33347320556641</v>
+        <v>29.5395622253418</v>
       </c>
     </row>
     <row r="101">
@@ -1235,7 +1235,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>35.16376495361328</v>
+        <v>29.53913879394531</v>
       </c>
     </row>
     <row r="102">
@@ -1243,7 +1243,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>35.34588623046875</v>
+        <v>29.5384693145752</v>
       </c>
     </row>
     <row r="103">
@@ -1251,7 +1251,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>35.25915145874023</v>
+        <v>29.53462219238281</v>
       </c>
     </row>
     <row r="104">
@@ -1259,7 +1259,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>34.98022079467773</v>
+        <v>29.53599548339844</v>
       </c>
     </row>
     <row r="105">
@@ -1267,7 +1267,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>34.74496078491211</v>
+        <v>29.53965950012207</v>
       </c>
     </row>
     <row r="106">
@@ -1275,7 +1275,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>34.61281585693359</v>
+        <v>29.53882789611816</v>
       </c>
     </row>
     <row r="107">
@@ -1283,7 +1283,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>34.89108657836914</v>
+        <v>29.53671264648438</v>
       </c>
     </row>
     <row r="108">
@@ -1291,7 +1291,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>35.40181350708008</v>
+        <v>29.53421783447266</v>
       </c>
     </row>
     <row r="109">
@@ -1299,7 +1299,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>35.64563369750977</v>
+        <v>29.53426742553711</v>
       </c>
     </row>
     <row r="110">
@@ -1307,7 +1307,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>35.00575637817383</v>
+        <v>29.55453872680664</v>
       </c>
     </row>
     <row r="111">
@@ -1315,7 +1315,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>35.04919052124023</v>
+        <v>29.56280517578125</v>
       </c>
     </row>
     <row r="112">
@@ -1323,7 +1323,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>35.32583618164062</v>
+        <v>29.57102203369141</v>
       </c>
     </row>
     <row r="113">
@@ -1331,7 +1331,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>35.27923202514648</v>
+        <v>29.56077194213867</v>
       </c>
     </row>
     <row r="114">
@@ -1339,7 +1339,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>35.38799285888672</v>
+        <v>29.56185531616211</v>
       </c>
     </row>
     <row r="115">
@@ -1347,7 +1347,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>34.90000915527344</v>
+        <v>29.56775283813477</v>
       </c>
     </row>
     <row r="116">
@@ -1355,7 +1355,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>34.81000137329102</v>
+        <v>29.57648086547852</v>
       </c>
     </row>
     <row r="117">
@@ -1363,7 +1363,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>34.56633758544922</v>
+        <v>29.58300018310547</v>
       </c>
     </row>
     <row r="118">
@@ -1371,7 +1371,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>34.87534713745117</v>
+        <v>29.57339859008789</v>
       </c>
     </row>
     <row r="119">
@@ -1379,7 +1379,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>34.89736175537109</v>
+        <v>29.57278060913086</v>
       </c>
     </row>
     <row r="120">
@@ -1387,7 +1387,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>34.97428894042969</v>
+        <v>29.56222724914551</v>
       </c>
     </row>
     <row r="121">
@@ -1395,7 +1395,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>35.17638778686523</v>
+        <v>29.55262756347656</v>
       </c>
     </row>
     <row r="122">
@@ -1403,7 +1403,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>34.96762466430664</v>
+        <v>29.57918167114258</v>
       </c>
     </row>
     <row r="123">
@@ -1411,7 +1411,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>34.76985549926758</v>
+        <v>29.58778190612793</v>
       </c>
     </row>
     <row r="124">
@@ -1419,7 +1419,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>34.7611198425293</v>
+        <v>29.59195518493652</v>
       </c>
     </row>
     <row r="125">
@@ -1427,7 +1427,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>34.82661819458008</v>
+        <v>29.59928512573242</v>
       </c>
     </row>
     <row r="126">
@@ -1435,7 +1435,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>34.88642501831055</v>
+        <v>29.59927940368652</v>
       </c>
     </row>
     <row r="127">
@@ -1443,7 +1443,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>34.93528366088867</v>
+        <v>29.60116195678711</v>
       </c>
     </row>
     <row r="128">
@@ -1451,7 +1451,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>34.9405632019043</v>
+        <v>29.60867881774902</v>
       </c>
     </row>
     <row r="129">
@@ -1459,7 +1459,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>34.83084106445312</v>
+        <v>29.61391830444336</v>
       </c>
     </row>
     <row r="130">
@@ -1467,7 +1467,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>34.839599609375</v>
+        <v>29.61504173278809</v>
       </c>
     </row>
     <row r="131">
@@ -1475,7 +1475,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>34.89757919311523</v>
+        <v>29.61175727844238</v>
       </c>
     </row>
     <row r="132">
@@ -1483,7 +1483,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>35.08428573608398</v>
+        <v>29.60580062866211</v>
       </c>
     </row>
     <row r="133">
@@ -1491,7 +1491,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>35.04377365112305</v>
+        <v>29.60788726806641</v>
       </c>
     </row>
     <row r="134">
@@ -1499,7 +1499,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>35.01158142089844</v>
+        <v>29.63205718994141</v>
       </c>
     </row>
     <row r="135">
@@ -1507,7 +1507,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>34.96546936035156</v>
+        <v>29.62810134887695</v>
       </c>
     </row>
     <row r="136">
@@ -1515,7 +1515,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>34.98917388916016</v>
+        <v>29.63400650024414</v>
       </c>
     </row>
     <row r="137">
@@ -1523,7 +1523,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>34.96121215820312</v>
+        <v>29.6302490234375</v>
       </c>
     </row>
     <row r="138">
@@ -1531,7 +1531,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>34.93304824829102</v>
+        <v>29.63152694702148</v>
       </c>
     </row>
     <row r="139">
@@ -1539,7 +1539,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>34.94417190551758</v>
+        <v>29.63182830810547</v>
       </c>
     </row>
     <row r="140">
@@ -1547,7 +1547,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>34.9085578918457</v>
+        <v>29.63180732727051</v>
       </c>
     </row>
     <row r="141">
@@ -1555,7 +1555,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>34.92389678955078</v>
+        <v>29.63422012329102</v>
       </c>
     </row>
     <row r="142">
@@ -1563,7 +1563,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>34.86384201049805</v>
+        <v>29.63458824157715</v>
       </c>
     </row>
     <row r="143">
@@ -1571,7 +1571,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>35.10906600952148</v>
+        <v>29.63575553894043</v>
       </c>
     </row>
     <row r="144">
@@ -1579,7 +1579,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>35.30815505981445</v>
+        <v>29.63569068908691</v>
       </c>
     </row>
     <row r="145">
@@ -1587,7 +1587,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>36.52506637573242</v>
+        <v>29.97015380859375</v>
       </c>
     </row>
     <row r="146">
@@ -1595,7 +1595,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>36.37200164794922</v>
+        <v>30.08426094055176</v>
       </c>
     </row>
     <row r="147">
@@ -1603,7 +1603,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>36.55903625488281</v>
+        <v>30.08163833618164</v>
       </c>
     </row>
     <row r="148">
@@ -1611,7 +1611,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>36.46026229858398</v>
+        <v>30.07111358642578</v>
       </c>
     </row>
     <row r="149">
@@ -1619,7 +1619,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>36.41917037963867</v>
+        <v>30.07704925537109</v>
       </c>
     </row>
     <row r="150">
@@ -1627,7 +1627,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>36.36628341674805</v>
+        <v>30.04824447631836</v>
       </c>
     </row>
     <row r="151">
@@ -1635,7 +1635,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>36.04610061645508</v>
+        <v>30.03113174438477</v>
       </c>
     </row>
     <row r="152">
@@ -1643,7 +1643,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>35.92256164550781</v>
+        <v>30.01424789428711</v>
       </c>
     </row>
     <row r="153">
@@ -1651,7 +1651,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>35.82793045043945</v>
+        <v>29.98085403442383</v>
       </c>
     </row>
     <row r="154">
@@ -1659,7 +1659,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>35.99526977539062</v>
+        <v>29.95633125305176</v>
       </c>
     </row>
     <row r="155">
@@ -1667,7 +1667,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>36.25240325927734</v>
+        <v>29.95291709899902</v>
       </c>
     </row>
     <row r="156">
@@ -1675,7 +1675,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>36.23968505859375</v>
+        <v>29.95378494262695</v>
       </c>
     </row>
     <row r="157">
@@ -1683,7 +1683,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>35.74512100219727</v>
+        <v>29.80228805541992</v>
       </c>
     </row>
     <row r="158">
@@ -1691,7 +1691,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>32.1833381652832</v>
+        <v>29.50712585449219</v>
       </c>
     </row>
     <row r="159">
@@ -1699,7 +1699,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>32.41276931762695</v>
+        <v>29.41272735595703</v>
       </c>
     </row>
     <row r="160">
@@ -1707,7 +1707,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>32.41291809082031</v>
+        <v>29.42043495178223</v>
       </c>
     </row>
     <row r="161">
@@ -1715,7 +1715,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>32.45869827270508</v>
+        <v>29.40922164916992</v>
       </c>
     </row>
     <row r="162">
@@ -1723,7 +1723,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>32.43112564086914</v>
+        <v>29.4440803527832</v>
       </c>
     </row>
     <row r="163">
@@ -1731,7 +1731,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>32.38488388061523</v>
+        <v>29.42203903198242</v>
       </c>
     </row>
     <row r="164">
@@ -1739,7 +1739,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>32.27078247070312</v>
+        <v>29.4024658203125</v>
       </c>
     </row>
     <row r="165">
@@ -1747,7 +1747,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>32.35664749145508</v>
+        <v>29.39289855957031</v>
       </c>
     </row>
     <row r="166">
@@ -1755,7 +1755,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>32.34420013427734</v>
+        <v>29.38922691345215</v>
       </c>
     </row>
     <row r="167">
@@ -1763,7 +1763,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>32.42222595214844</v>
+        <v>29.41864013671875</v>
       </c>
     </row>
     <row r="168">
@@ -1771,7 +1771,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>32.40280151367188</v>
+        <v>29.48266220092773</v>
       </c>
     </row>
     <row r="169">
@@ -1779,7 +1779,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>32.33364868164062</v>
+        <v>29.48379898071289</v>
       </c>
     </row>
     <row r="170">
@@ -1787,7 +1787,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>32.2269287109375</v>
+        <v>29.51852798461914</v>
       </c>
     </row>
     <row r="171">
@@ -1795,7 +1795,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>32.37585067749023</v>
+        <v>29.52440643310547</v>
       </c>
     </row>
     <row r="172">
@@ -1803,7 +1803,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>32.33876800537109</v>
+        <v>29.55359649658203</v>
       </c>
     </row>
     <row r="173">
@@ -1811,7 +1811,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>32.2612190246582</v>
+        <v>29.53870010375977</v>
       </c>
     </row>
     <row r="174">
@@ -1819,7 +1819,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>32.17327117919922</v>
+        <v>29.49727630615234</v>
       </c>
     </row>
     <row r="175">
@@ -1827,7 +1827,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>32.26708984375</v>
+        <v>29.5306282043457</v>
       </c>
     </row>
     <row r="176">
@@ -1835,7 +1835,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>32.48893737792969</v>
+        <v>29.55595016479492</v>
       </c>
     </row>
     <row r="177">
@@ -1843,7 +1843,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>32.34432220458984</v>
+        <v>29.55588531494141</v>
       </c>
     </row>
     <row r="178">
@@ -1851,7 +1851,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>32.20707321166992</v>
+        <v>29.60668563842773</v>
       </c>
     </row>
     <row r="179">
@@ -1859,7 +1859,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>32.39858245849609</v>
+        <v>29.62090873718262</v>
       </c>
     </row>
     <row r="180">
@@ -1867,7 +1867,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>32.8764762878418</v>
+        <v>29.5913257598877</v>
       </c>
     </row>
     <row r="181">
@@ -1875,7 +1875,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>33.05454635620117</v>
+        <v>29.66176986694336</v>
       </c>
     </row>
     <row r="182">
@@ -1883,7 +1883,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>32.15816116333008</v>
+        <v>29.66056823730469</v>
       </c>
     </row>
     <row r="183">
@@ -1891,7 +1891,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>31.90730285644531</v>
+        <v>29.63182830810547</v>
       </c>
     </row>
     <row r="184">
@@ -1899,7 +1899,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>32.11065292358398</v>
+        <v>29.62772750854492</v>
       </c>
     </row>
     <row r="185">
@@ -1907,7 +1907,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>31.8183479309082</v>
+        <v>29.66976547241211</v>
       </c>
     </row>
     <row r="186">
@@ -1915,7 +1915,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>33.27792739868164</v>
+        <v>29.71020698547363</v>
       </c>
     </row>
     <row r="187">
@@ -1923,7 +1923,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>32.05787658691406</v>
+        <v>29.68038940429688</v>
       </c>
     </row>
     <row r="188">
@@ -1931,7 +1931,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>31.77146148681641</v>
+        <v>29.61739349365234</v>
       </c>
     </row>
     <row r="189">
@@ -1939,7 +1939,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>31.60300827026367</v>
+        <v>29.56663131713867</v>
       </c>
     </row>
     <row r="190">
@@ -1947,7 +1947,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>31.62470054626465</v>
+        <v>29.53877258300781</v>
       </c>
     </row>
     <row r="191">
@@ -1955,7 +1955,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>31.68529510498047</v>
+        <v>29.5191764831543</v>
       </c>
     </row>
     <row r="192">
@@ -1963,7 +1963,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>31.67991256713867</v>
+        <v>29.52312469482422</v>
       </c>
     </row>
     <row r="193">
@@ -1971,7 +1971,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>31.60589218139648</v>
+        <v>29.47300338745117</v>
       </c>
     </row>
     <row r="194">
@@ -1979,7 +1979,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>31.36698913574219</v>
+        <v>29.26471710205078</v>
       </c>
     </row>
     <row r="195">
@@ -1987,7 +1987,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>31.32351493835449</v>
+        <v>29.19709205627441</v>
       </c>
     </row>
     <row r="196">
@@ -1995,7 +1995,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>31.23138809204102</v>
+        <v>29.19665336608887</v>
       </c>
     </row>
     <row r="197">
@@ -2003,7 +2003,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>31.17805862426758</v>
+        <v>29.18464660644531</v>
       </c>
     </row>
     <row r="198">
@@ -2011,7 +2011,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>31.36339569091797</v>
+        <v>29.18500137329102</v>
       </c>
     </row>
     <row r="199">
@@ -2019,7 +2019,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>31.05180168151855</v>
+        <v>29.1729621887207</v>
       </c>
     </row>
     <row r="200">
@@ -2027,7 +2027,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>31.07701301574707</v>
+        <v>29.17534065246582</v>
       </c>
     </row>
     <row r="201">
@@ -2035,7 +2035,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>31.12229156494141</v>
+        <v>29.17294692993164</v>
       </c>
     </row>
     <row r="202">
@@ -2043,7 +2043,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="n">
-        <v>31.18671226501465</v>
+        <v>29.17933654785156</v>
       </c>
     </row>
     <row r="203">
@@ -2051,7 +2051,7 @@
         <v>201</v>
       </c>
       <c r="B203" t="n">
-        <v>31.04788970947266</v>
+        <v>29.16879653930664</v>
       </c>
     </row>
     <row r="204">
@@ -2059,7 +2059,7 @@
         <v>202</v>
       </c>
       <c r="B204" t="n">
-        <v>31.30196952819824</v>
+        <v>29.17822265625</v>
       </c>
     </row>
     <row r="205">
@@ -2067,7 +2067,7 @@
         <v>203</v>
       </c>
       <c r="B205" t="n">
-        <v>31.18180274963379</v>
+        <v>29.17443466186523</v>
       </c>
     </row>
     <row r="206">
@@ -2075,7 +2075,7 @@
         <v>204</v>
       </c>
       <c r="B206" t="n">
-        <v>31.25729560852051</v>
+        <v>29.17940521240234</v>
       </c>
     </row>
     <row r="207">
@@ -2083,7 +2083,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="n">
-        <v>31.09253311157227</v>
+        <v>29.16066741943359</v>
       </c>
     </row>
     <row r="208">
@@ -2091,7 +2091,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="n">
-        <v>31.09857559204102</v>
+        <v>29.17122650146484</v>
       </c>
     </row>
     <row r="209">
@@ -2099,7 +2099,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="n">
-        <v>31.11600112915039</v>
+        <v>29.17301559448242</v>
       </c>
     </row>
     <row r="210">
@@ -2107,7 +2107,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="n">
-        <v>31.06384658813477</v>
+        <v>29.15933799743652</v>
       </c>
     </row>
     <row r="211">
@@ -2115,7 +2115,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="n">
-        <v>30.9882698059082</v>
+        <v>29.15320587158203</v>
       </c>
     </row>
     <row r="212">
@@ -2123,7 +2123,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="n">
-        <v>31.00506401062012</v>
+        <v>29.15938949584961</v>
       </c>
     </row>
     <row r="213">
@@ -2131,7 +2131,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="n">
-        <v>30.90150260925293</v>
+        <v>29.16012954711914</v>
       </c>
     </row>
     <row r="214">
@@ -2139,7 +2139,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="n">
-        <v>30.89618873596191</v>
+        <v>29.18147659301758</v>
       </c>
     </row>
     <row r="215">
@@ -2147,7 +2147,7 @@
         <v>213</v>
       </c>
       <c r="B215" t="n">
-        <v>31.15330505371094</v>
+        <v>29.20072555541992</v>
       </c>
     </row>
     <row r="216">
@@ -2155,7 +2155,7 @@
         <v>214</v>
       </c>
       <c r="B216" t="n">
-        <v>31.12917137145996</v>
+        <v>29.20310974121094</v>
       </c>
     </row>
     <row r="217">
@@ -2163,7 +2163,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="n">
-        <v>31.12652206420898</v>
+        <v>29.17868995666504</v>
       </c>
     </row>
     <row r="218">
@@ -2171,7 +2171,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="n">
-        <v>31.06136322021484</v>
+        <v>29.17657089233398</v>
       </c>
     </row>
     <row r="219">
@@ -2179,7 +2179,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="n">
-        <v>30.87492561340332</v>
+        <v>29.16193008422852</v>
       </c>
     </row>
     <row r="220">
@@ -2187,7 +2187,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="n">
-        <v>31.08648872375488</v>
+        <v>29.16691207885742</v>
       </c>
     </row>
     <row r="221">
@@ -2195,7 +2195,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="n">
-        <v>30.91025924682617</v>
+        <v>29.16000366210938</v>
       </c>
     </row>
     <row r="222">
@@ -2203,7 +2203,7 @@
         <v>220</v>
       </c>
       <c r="B222" t="n">
-        <v>30.78577995300293</v>
+        <v>29.15751838684082</v>
       </c>
     </row>
     <row r="223">
@@ -2211,7 +2211,7 @@
         <v>221</v>
       </c>
       <c r="B223" t="n">
-        <v>30.80229949951172</v>
+        <v>29.16596221923828</v>
       </c>
     </row>
     <row r="224">
@@ -2219,7 +2219,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="n">
-        <v>30.55086135864258</v>
+        <v>29.17024803161621</v>
       </c>
     </row>
     <row r="225">
@@ -2227,7 +2227,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="n">
-        <v>30.64284515380859</v>
+        <v>29.17029571533203</v>
       </c>
     </row>
     <row r="226">
@@ -2235,7 +2235,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="n">
-        <v>30.00007247924805</v>
+        <v>29.14741325378418</v>
       </c>
     </row>
     <row r="227">
@@ -2243,7 +2243,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="n">
-        <v>30.09125900268555</v>
+        <v>29.15628814697266</v>
       </c>
     </row>
     <row r="228">
@@ -2251,7 +2251,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="n">
-        <v>30.1221981048584</v>
+        <v>29.16621398925781</v>
       </c>
     </row>
     <row r="229">
@@ -2259,7 +2259,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="n">
-        <v>30.07226943969727</v>
+        <v>29.17862129211426</v>
       </c>
     </row>
     <row r="230">
@@ -2267,7 +2267,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="n">
-        <v>29.98798751831055</v>
+        <v>29.17065620422363</v>
       </c>
     </row>
     <row r="231">
@@ -2275,7 +2275,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="n">
-        <v>29.98380279541016</v>
+        <v>29.17271041870117</v>
       </c>
     </row>
     <row r="232">
@@ -2283,7 +2283,7 @@
         <v>230</v>
       </c>
       <c r="B232" t="n">
-        <v>29.84786987304688</v>
+        <v>29.17790222167969</v>
       </c>
     </row>
     <row r="233">
@@ -2291,7 +2291,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="n">
-        <v>29.88484573364258</v>
+        <v>29.17847442626953</v>
       </c>
     </row>
     <row r="234">
@@ -2299,7 +2299,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="n">
-        <v>29.91114044189453</v>
+        <v>29.17941093444824</v>
       </c>
     </row>
     <row r="235">
@@ -2307,7 +2307,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="n">
-        <v>29.88680267333984</v>
+        <v>29.18082809448242</v>
       </c>
     </row>
     <row r="236">
@@ -2315,7 +2315,7 @@
         <v>234</v>
       </c>
       <c r="B236" t="n">
-        <v>29.63205528259277</v>
+        <v>29.18368530273438</v>
       </c>
     </row>
     <row r="237">
@@ -2323,7 +2323,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="n">
-        <v>29.46484375</v>
+        <v>29.18660736083984</v>
       </c>
     </row>
     <row r="238">
@@ -2331,7 +2331,7 @@
         <v>236</v>
       </c>
       <c r="B238" t="n">
-        <v>29.60452079772949</v>
+        <v>29.19918823242188</v>
       </c>
     </row>
     <row r="239">
@@ -2339,7 +2339,7 @@
         <v>237</v>
       </c>
       <c r="B239" t="n">
-        <v>29.53532791137695</v>
+        <v>29.19021987915039</v>
       </c>
     </row>
     <row r="240">
@@ -2347,7 +2347,7 @@
         <v>238</v>
       </c>
       <c r="B240" t="n">
-        <v>29.64433097839355</v>
+        <v>29.18857955932617</v>
       </c>
     </row>
     <row r="241">
@@ -2355,7 +2355,7 @@
         <v>239</v>
       </c>
       <c r="B241" t="n">
-        <v>29.59354019165039</v>
+        <v>29.20088577270508</v>
       </c>
     </row>
     <row r="242">
@@ -2363,7 +2363,7 @@
         <v>240</v>
       </c>
       <c r="B242" t="n">
-        <v>29.50828552246094</v>
+        <v>29.20301818847656</v>
       </c>
     </row>
     <row r="243">
@@ -2371,7 +2371,7 @@
         <v>241</v>
       </c>
       <c r="B243" t="n">
-        <v>29.52009963989258</v>
+        <v>29.19091415405273</v>
       </c>
     </row>
     <row r="244">
@@ -2379,7 +2379,7 @@
         <v>242</v>
       </c>
       <c r="B244" t="n">
-        <v>29.47703742980957</v>
+        <v>29.20420455932617</v>
       </c>
     </row>
     <row r="245">
@@ -2387,7 +2387,7 @@
         <v>243</v>
       </c>
       <c r="B245" t="n">
-        <v>29.44343948364258</v>
+        <v>29.23194694519043</v>
       </c>
     </row>
     <row r="246">
@@ -2395,7 +2395,7 @@
         <v>244</v>
       </c>
       <c r="B246" t="n">
-        <v>29.35552215576172</v>
+        <v>29.20661926269531</v>
       </c>
     </row>
     <row r="247">
@@ -2403,7 +2403,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="n">
-        <v>29.31406593322754</v>
+        <v>29.20034027099609</v>
       </c>
     </row>
     <row r="248">
@@ -2411,7 +2411,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="n">
-        <v>29.28513336181641</v>
+        <v>29.20584869384766</v>
       </c>
     </row>
     <row r="249">
@@ -2419,7 +2419,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="n">
-        <v>29.2425708770752</v>
+        <v>29.2000617980957</v>
       </c>
     </row>
     <row r="250">
@@ -2427,7 +2427,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="n">
-        <v>29.54878425598145</v>
+        <v>29.1929817199707</v>
       </c>
     </row>
     <row r="251">
@@ -2435,7 +2435,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="n">
-        <v>29.4244270324707</v>
+        <v>29.19566535949707</v>
       </c>
     </row>
     <row r="252">
@@ -2443,7 +2443,7 @@
         <v>250</v>
       </c>
       <c r="B252" t="n">
-        <v>29.23567199707031</v>
+        <v>29.19456100463867</v>
       </c>
     </row>
     <row r="253">
@@ -2451,7 +2451,7 @@
         <v>251</v>
       </c>
       <c r="B253" t="n">
-        <v>29.45842742919922</v>
+        <v>29.20210456848145</v>
       </c>
     </row>
     <row r="254">
@@ -2459,7 +2459,7 @@
         <v>252</v>
       </c>
       <c r="B254" t="n">
-        <v>29.26629257202148</v>
+        <v>29.21118927001953</v>
       </c>
     </row>
     <row r="255">
@@ -2467,7 +2467,7 @@
         <v>253</v>
       </c>
       <c r="B255" t="n">
-        <v>30.09063148498535</v>
+        <v>29.22881317138672</v>
       </c>
     </row>
     <row r="256">
@@ -2475,7 +2475,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="n">
-        <v>30.32679748535156</v>
+        <v>29.33320426940918</v>
       </c>
     </row>
     <row r="257">
@@ -2483,7 +2483,7 @@
         <v>255</v>
       </c>
       <c r="B257" t="n">
-        <v>30.24397087097168</v>
+        <v>29.35150146484375</v>
       </c>
     </row>
     <row r="258">
@@ -2491,7 +2491,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="n">
-        <v>30.3016357421875</v>
+        <v>29.35662078857422</v>
       </c>
     </row>
     <row r="259">
@@ -2499,7 +2499,7 @@
         <v>257</v>
       </c>
       <c r="B259" t="n">
-        <v>30.26596069335938</v>
+        <v>29.38817596435547</v>
       </c>
     </row>
     <row r="260">
@@ -2507,7 +2507,7 @@
         <v>258</v>
       </c>
       <c r="B260" t="n">
-        <v>30.02081298828125</v>
+        <v>29.36079025268555</v>
       </c>
     </row>
     <row r="261">
@@ -2515,7 +2515,7 @@
         <v>259</v>
       </c>
       <c r="B261" t="n">
-        <v>30.25124740600586</v>
+        <v>29.36072540283203</v>
       </c>
     </row>
     <row r="262">
@@ -2523,7 +2523,7 @@
         <v>260</v>
       </c>
       <c r="B262" t="n">
-        <v>29.87490272521973</v>
+        <v>29.39090538024902</v>
       </c>
     </row>
     <row r="263">
@@ -2531,7 +2531,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="n">
-        <v>29.62726402282715</v>
+        <v>29.45476531982422</v>
       </c>
     </row>
     <row r="264">
@@ -2539,7 +2539,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="n">
-        <v>29.71913528442383</v>
+        <v>29.46817779541016</v>
       </c>
     </row>
     <row r="265">
@@ -2547,7 +2547,7 @@
         <v>263</v>
       </c>
       <c r="B265" t="n">
-        <v>29.40591239929199</v>
+        <v>29.48938941955566</v>
       </c>
     </row>
     <row r="266">
@@ -2555,7 +2555,7 @@
         <v>264</v>
       </c>
       <c r="B266" t="n">
-        <v>29.42016220092773</v>
+        <v>29.51585006713867</v>
       </c>
     </row>
     <row r="267">
@@ -2563,7 +2563,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="n">
-        <v>29.28741455078125</v>
+        <v>29.56736183166504</v>
       </c>
     </row>
     <row r="268">
@@ -2571,7 +2571,7 @@
         <v>266</v>
       </c>
       <c r="B268" t="n">
-        <v>29.35325050354004</v>
+        <v>29.56352996826172</v>
       </c>
     </row>
     <row r="269">
@@ -2579,7 +2579,7 @@
         <v>267</v>
       </c>
       <c r="B269" t="n">
-        <v>29.09295272827148</v>
+        <v>29.59676742553711</v>
       </c>
     </row>
     <row r="270">
@@ -2587,7 +2587,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="n">
-        <v>28.76417922973633</v>
+        <v>29.66744232177734</v>
       </c>
     </row>
     <row r="271">
@@ -2595,7 +2595,7 @@
         <v>269</v>
       </c>
       <c r="B271" t="n">
-        <v>28.44443893432617</v>
+        <v>29.70965194702148</v>
       </c>
     </row>
     <row r="272">
@@ -2603,7 +2603,7 @@
         <v>270</v>
       </c>
       <c r="B272" t="n">
-        <v>28.85575103759766</v>
+        <v>29.66504669189453</v>
       </c>
     </row>
     <row r="273">
@@ -2611,7 +2611,7 @@
         <v>271</v>
       </c>
       <c r="B273" t="n">
-        <v>28.70179748535156</v>
+        <v>29.7267951965332</v>
       </c>
     </row>
     <row r="274">
@@ -2619,7 +2619,7 @@
         <v>272</v>
       </c>
       <c r="B274" t="n">
-        <v>28.86921691894531</v>
+        <v>29.68653297424316</v>
       </c>
     </row>
     <row r="275">
@@ -2627,7 +2627,7 @@
         <v>273</v>
       </c>
       <c r="B275" t="n">
-        <v>28.50929641723633</v>
+        <v>29.65428924560547</v>
       </c>
     </row>
     <row r="276">
@@ -2635,7 +2635,7 @@
         <v>274</v>
       </c>
       <c r="B276" t="n">
-        <v>29.37727737426758</v>
+        <v>29.64315032958984</v>
       </c>
     </row>
     <row r="277">
@@ -2643,7 +2643,7 @@
         <v>275</v>
       </c>
       <c r="B277" t="n">
-        <v>29.37017822265625</v>
+        <v>29.64597702026367</v>
       </c>
     </row>
     <row r="278">
@@ -2651,7 +2651,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="n">
-        <v>29.35660171508789</v>
+        <v>29.70496368408203</v>
       </c>
     </row>
     <row r="279">
@@ -2659,7 +2659,7 @@
         <v>277</v>
       </c>
       <c r="B279" t="n">
-        <v>29.39867782592773</v>
+        <v>29.58512115478516</v>
       </c>
     </row>
     <row r="280">
@@ -2667,7 +2667,7 @@
         <v>278</v>
       </c>
       <c r="B280" t="n">
-        <v>29.35815811157227</v>
+        <v>29.61361503601074</v>
       </c>
     </row>
     <row r="281">
@@ -2675,7 +2675,7 @@
         <v>279</v>
       </c>
       <c r="B281" t="n">
-        <v>29.36886215209961</v>
+        <v>29.67767906188965</v>
       </c>
     </row>
     <row r="282">
@@ -2683,7 +2683,7 @@
         <v>280</v>
       </c>
       <c r="B282" t="n">
-        <v>28.42769813537598</v>
+        <v>29.75461196899414</v>
       </c>
     </row>
     <row r="283">
@@ -2691,7 +2691,7 @@
         <v>281</v>
       </c>
       <c r="B283" t="n">
-        <v>28.22341918945312</v>
+        <v>29.72367858886719</v>
       </c>
     </row>
     <row r="284">
@@ -2699,7 +2699,7 @@
         <v>282</v>
       </c>
       <c r="B284" t="n">
-        <v>28.33340454101562</v>
+        <v>29.68420791625977</v>
       </c>
     </row>
     <row r="285">
@@ -2707,7 +2707,7 @@
         <v>283</v>
       </c>
       <c r="B285" t="n">
-        <v>28.19156837463379</v>
+        <v>29.7208137512207</v>
       </c>
     </row>
     <row r="286">
@@ -2715,7 +2715,7 @@
         <v>284</v>
       </c>
       <c r="B286" t="n">
-        <v>28.30814361572266</v>
+        <v>29.71746826171875</v>
       </c>
     </row>
     <row r="287">
@@ -2723,7 +2723,7 @@
         <v>285</v>
       </c>
       <c r="B287" t="n">
-        <v>28.26990127563477</v>
+        <v>29.82780075073242</v>
       </c>
     </row>
     <row r="288">
@@ -2731,7 +2731,7 @@
         <v>286</v>
       </c>
       <c r="B288" t="n">
-        <v>28.24674224853516</v>
+        <v>29.8079833984375</v>
       </c>
     </row>
     <row r="289">
@@ -2739,7 +2739,7 @@
         <v>287</v>
       </c>
       <c r="B289" t="n">
-        <v>28.05838775634766</v>
+        <v>29.75414276123047</v>
       </c>
     </row>
     <row r="290">
@@ -2747,7 +2747,7 @@
         <v>288</v>
       </c>
       <c r="B290" t="n">
-        <v>28.15464210510254</v>
+        <v>29.76490020751953</v>
       </c>
     </row>
     <row r="291">
@@ -2755,7 +2755,7 @@
         <v>289</v>
       </c>
       <c r="B291" t="n">
-        <v>28.05050659179688</v>
+        <v>29.78067779541016</v>
       </c>
     </row>
     <row r="292">
@@ -2763,7 +2763,7 @@
         <v>290</v>
       </c>
       <c r="B292" t="n">
-        <v>28.18222808837891</v>
+        <v>29.84264755249023</v>
       </c>
     </row>
     <row r="293">
@@ -2771,7 +2771,7 @@
         <v>291</v>
       </c>
       <c r="B293" t="n">
-        <v>28.09691047668457</v>
+        <v>29.83902931213379</v>
       </c>
     </row>
     <row r="294">
@@ -2779,7 +2779,7 @@
         <v>292</v>
       </c>
       <c r="B294" t="n">
-        <v>28.18478012084961</v>
+        <v>29.87514114379883</v>
       </c>
     </row>
     <row r="295">
@@ -2787,7 +2787,7 @@
         <v>293</v>
       </c>
       <c r="B295" t="n">
-        <v>28.23150253295898</v>
+        <v>29.86191940307617</v>
       </c>
     </row>
     <row r="296">
@@ -2795,7 +2795,7 @@
         <v>294</v>
       </c>
       <c r="B296" t="n">
-        <v>28.08763885498047</v>
+        <v>29.85811996459961</v>
       </c>
     </row>
     <row r="297">
@@ -2803,7 +2803,7 @@
         <v>295</v>
       </c>
       <c r="B297" t="n">
-        <v>28.07855224609375</v>
+        <v>29.8144416809082</v>
       </c>
     </row>
     <row r="298">
@@ -2811,7 +2811,7 @@
         <v>296</v>
       </c>
       <c r="B298" t="n">
-        <v>28.18966865539551</v>
+        <v>29.83750152587891</v>
       </c>
     </row>
     <row r="299">
@@ -2819,7 +2819,7 @@
         <v>297</v>
       </c>
       <c r="B299" t="n">
-        <v>28.61426544189453</v>
+        <v>29.89747619628906</v>
       </c>
     </row>
     <row r="300">
@@ -2827,7 +2827,7 @@
         <v>298</v>
       </c>
       <c r="B300" t="n">
-        <v>28.69968223571777</v>
+        <v>29.9190616607666</v>
       </c>
     </row>
     <row r="301">
@@ -2835,7 +2835,7 @@
         <v>299</v>
       </c>
       <c r="B301" t="n">
-        <v>28.47898292541504</v>
+        <v>29.8762321472168</v>
       </c>
     </row>
     <row r="302">
@@ -2843,7 +2843,7 @@
         <v>300</v>
       </c>
       <c r="B302" t="n">
-        <v>28.41509628295898</v>
+        <v>29.88778305053711</v>
       </c>
     </row>
     <row r="303">
@@ -2851,7 +2851,7 @@
         <v>301</v>
       </c>
       <c r="B303" t="n">
-        <v>28.5508918762207</v>
+        <v>29.90366744995117</v>
       </c>
     </row>
     <row r="304">
@@ -2859,7 +2859,7 @@
         <v>302</v>
       </c>
       <c r="B304" t="n">
-        <v>28.20731735229492</v>
+        <v>29.97427368164062</v>
       </c>
     </row>
     <row r="305">
@@ -2867,7 +2867,7 @@
         <v>303</v>
       </c>
       <c r="B305" t="n">
-        <v>28.10228538513184</v>
+        <v>30.01302909851074</v>
       </c>
     </row>
     <row r="306">
@@ -2875,7 +2875,7 @@
         <v>304</v>
       </c>
       <c r="B306" t="n">
-        <v>28.30769538879395</v>
+        <v>29.98503875732422</v>
       </c>
     </row>
     <row r="307">
@@ -2883,7 +2883,7 @@
         <v>305</v>
       </c>
       <c r="B307" t="n">
-        <v>28.45722961425781</v>
+        <v>29.93022918701172</v>
       </c>
     </row>
     <row r="308">
@@ -2891,7 +2891,7 @@
         <v>306</v>
       </c>
       <c r="B308" t="n">
-        <v>28.52532958984375</v>
+        <v>29.89963531494141</v>
       </c>
     </row>
     <row r="309">
@@ -2899,7 +2899,7 @@
         <v>307</v>
       </c>
       <c r="B309" t="n">
-        <v>28.51432800292969</v>
+        <v>29.88398170471191</v>
       </c>
     </row>
     <row r="310">
@@ -2907,7 +2907,7 @@
         <v>308</v>
       </c>
       <c r="B310" t="n">
-        <v>28.6756591796875</v>
+        <v>29.94882583618164</v>
       </c>
     </row>
     <row r="311">
@@ -2915,7 +2915,7 @@
         <v>309</v>
       </c>
       <c r="B311" t="n">
-        <v>28.52313232421875</v>
+        <v>30.04490661621094</v>
       </c>
     </row>
     <row r="312">
@@ -2923,7 +2923,7 @@
         <v>310</v>
       </c>
       <c r="B312" t="n">
-        <v>28.30676651000977</v>
+        <v>30.0107536315918</v>
       </c>
     </row>
     <row r="313">
@@ -2931,7 +2931,7 @@
         <v>311</v>
       </c>
       <c r="B313" t="n">
-        <v>28.26626205444336</v>
+        <v>30.00839614868164</v>
       </c>
     </row>
     <row r="314">
@@ -2939,7 +2939,7 @@
         <v>312</v>
       </c>
       <c r="B314" t="n">
-        <v>28.25146102905273</v>
+        <v>30.04351806640625</v>
       </c>
     </row>
     <row r="315">
@@ -2947,7 +2947,7 @@
         <v>313</v>
       </c>
       <c r="B315" t="n">
-        <v>28.03663444519043</v>
+        <v>30.15995025634766</v>
       </c>
     </row>
     <row r="316">
@@ -2955,7 +2955,7 @@
         <v>314</v>
       </c>
       <c r="B316" t="n">
-        <v>28.06655883789062</v>
+        <v>30.12856674194336</v>
       </c>
     </row>
     <row r="317">
@@ -2963,7 +2963,7 @@
         <v>315</v>
       </c>
       <c r="B317" t="n">
-        <v>28.11641311645508</v>
+        <v>30.12262725830078</v>
       </c>
     </row>
     <row r="318">
@@ -2971,7 +2971,7 @@
         <v>316</v>
       </c>
       <c r="B318" t="n">
-        <v>28.55300903320312</v>
+        <v>30.04008865356445</v>
       </c>
     </row>
     <row r="319">
@@ -2979,7 +2979,7 @@
         <v>317</v>
       </c>
       <c r="B319" t="n">
-        <v>28.59901809692383</v>
+        <v>30.03997421264648</v>
       </c>
     </row>
     <row r="320">
@@ -2987,7 +2987,7 @@
         <v>318</v>
       </c>
       <c r="B320" t="n">
-        <v>28.48945999145508</v>
+        <v>30.09147262573242</v>
       </c>
     </row>
     <row r="321">
@@ -2995,7 +2995,7 @@
         <v>319</v>
       </c>
       <c r="B321" t="n">
-        <v>28.14593124389648</v>
+        <v>30.0923900604248</v>
       </c>
     </row>
     <row r="322">
@@ -3003,7 +3003,7 @@
         <v>320</v>
       </c>
       <c r="B322" t="n">
-        <v>28.31051063537598</v>
+        <v>30.06559181213379</v>
       </c>
     </row>
     <row r="323">
@@ -3011,7 +3011,7 @@
         <v>321</v>
       </c>
       <c r="B323" t="n">
-        <v>28.46016502380371</v>
+        <v>30.16938400268555</v>
       </c>
     </row>
     <row r="324">
@@ -3019,7 +3019,7 @@
         <v>322</v>
       </c>
       <c r="B324" t="n">
-        <v>28.31880378723145</v>
+        <v>30.18485450744629</v>
       </c>
     </row>
     <row r="325">
@@ -3027,7 +3027,7 @@
         <v>323</v>
       </c>
       <c r="B325" t="n">
-        <v>27.68955230712891</v>
+        <v>30.24246597290039</v>
       </c>
     </row>
     <row r="326">
@@ -3035,7 +3035,7 @@
         <v>324</v>
       </c>
       <c r="B326" t="n">
-        <v>27.61528396606445</v>
+        <v>30.25394058227539</v>
       </c>
     </row>
     <row r="327">
@@ -3043,7 +3043,7 @@
         <v>325</v>
       </c>
       <c r="B327" t="n">
-        <v>27.72673225402832</v>
+        <v>30.29187965393066</v>
       </c>
     </row>
     <row r="328">
@@ -3051,7 +3051,7 @@
         <v>326</v>
       </c>
       <c r="B328" t="n">
-        <v>27.78463745117188</v>
+        <v>30.43586730957031</v>
       </c>
     </row>
     <row r="329">
@@ -3059,7 +3059,7 @@
         <v>327</v>
       </c>
       <c r="B329" t="n">
-        <v>27.70291709899902</v>
+        <v>30.34625816345215</v>
       </c>
     </row>
     <row r="330">
@@ -3067,7 +3067,7 @@
         <v>328</v>
       </c>
       <c r="B330" t="n">
-        <v>27.841796875</v>
+        <v>30.30902862548828</v>
       </c>
     </row>
     <row r="331">
@@ -3075,7 +3075,7 @@
         <v>329</v>
       </c>
       <c r="B331" t="n">
-        <v>27.70424270629883</v>
+        <v>30.31364059448242</v>
       </c>
     </row>
     <row r="332">
@@ -3083,7 +3083,7 @@
         <v>330</v>
       </c>
       <c r="B332" t="n">
-        <v>27.47711181640625</v>
+        <v>30.24309158325195</v>
       </c>
     </row>
     <row r="333">
@@ -3091,7 +3091,7 @@
         <v>331</v>
       </c>
       <c r="B333" t="n">
-        <v>27.26907730102539</v>
+        <v>30.29067230224609</v>
       </c>
     </row>
     <row r="334">
@@ -3099,7 +3099,7 @@
         <v>332</v>
       </c>
       <c r="B334" t="n">
-        <v>27.54189300537109</v>
+        <v>30.38537979125977</v>
       </c>
     </row>
     <row r="335">
@@ -3107,7 +3107,7 @@
         <v>333</v>
       </c>
       <c r="B335" t="n">
-        <v>27.90285491943359</v>
+        <v>30.42660140991211</v>
       </c>
     </row>
     <row r="336">
@@ -3115,7 +3115,7 @@
         <v>334</v>
       </c>
       <c r="B336" t="n">
-        <v>27.75692749023438</v>
+        <v>30.42813491821289</v>
       </c>
     </row>
     <row r="337">
@@ -3123,7 +3123,7 @@
         <v>335</v>
       </c>
       <c r="B337" t="n">
-        <v>27.34747886657715</v>
+        <v>30.42011260986328</v>
       </c>
     </row>
     <row r="338">
@@ -3131,7 +3131,7 @@
         <v>336</v>
       </c>
       <c r="B338" t="n">
-        <v>27.43218994140625</v>
+        <v>30.42666053771973</v>
       </c>
     </row>
     <row r="339">
@@ -3139,7 +3139,7 @@
         <v>337</v>
       </c>
       <c r="B339" t="n">
-        <v>27.27855682373047</v>
+        <v>30.4537181854248</v>
       </c>
     </row>
     <row r="340">
@@ -3147,7 +3147,7 @@
         <v>338</v>
       </c>
       <c r="B340" t="n">
-        <v>27.36021614074707</v>
+        <v>30.45418930053711</v>
       </c>
     </row>
     <row r="341">
@@ -3155,7 +3155,7 @@
         <v>339</v>
       </c>
       <c r="B341" t="n">
-        <v>27.39453125</v>
+        <v>30.42098045349121</v>
       </c>
     </row>
     <row r="342">
@@ -3163,7 +3163,7 @@
         <v>340</v>
       </c>
       <c r="B342" t="n">
-        <v>27.32286834716797</v>
+        <v>30.40694427490234</v>
       </c>
     </row>
     <row r="343">
@@ -3171,7 +3171,7 @@
         <v>341</v>
       </c>
       <c r="B343" t="n">
-        <v>27.3377513885498</v>
+        <v>30.40519714355469</v>
       </c>
     </row>
     <row r="344">
@@ -3179,7 +3179,7 @@
         <v>342</v>
       </c>
       <c r="B344" t="n">
-        <v>27.39561462402344</v>
+        <v>30.36823272705078</v>
       </c>
     </row>
     <row r="345">
@@ -3187,7 +3187,7 @@
         <v>343</v>
       </c>
       <c r="B345" t="n">
-        <v>27.34330749511719</v>
+        <v>30.45326995849609</v>
       </c>
     </row>
     <row r="346">
@@ -3195,7 +3195,7 @@
         <v>344</v>
       </c>
       <c r="B346" t="n">
-        <v>27.57090377807617</v>
+        <v>30.45399284362793</v>
       </c>
     </row>
     <row r="347">
@@ -3203,7 +3203,7 @@
         <v>345</v>
       </c>
       <c r="B347" t="n">
-        <v>28.0280876159668</v>
+        <v>30.45491027832031</v>
       </c>
     </row>
     <row r="348">
@@ -3211,7 +3211,7 @@
         <v>346</v>
       </c>
       <c r="B348" t="n">
-        <v>28.1966552734375</v>
+        <v>30.45571517944336</v>
       </c>
     </row>
     <row r="349">
@@ -3219,7 +3219,7 @@
         <v>347</v>
       </c>
       <c r="B349" t="n">
-        <v>28.36489486694336</v>
+        <v>30.45702743530273</v>
       </c>
     </row>
     <row r="350">
@@ -3227,7 +3227,7 @@
         <v>348</v>
       </c>
       <c r="B350" t="n">
-        <v>28.45219993591309</v>
+        <v>30.45573425292969</v>
       </c>
     </row>
     <row r="351">
@@ -3235,7 +3235,7 @@
         <v>349</v>
       </c>
       <c r="B351" t="n">
-        <v>28.44845390319824</v>
+        <v>30.46197509765625</v>
       </c>
     </row>
     <row r="352">
@@ -3243,7 +3243,7 @@
         <v>350</v>
       </c>
       <c r="B352" t="n">
-        <v>28.43437194824219</v>
+        <v>30.46620178222656</v>
       </c>
     </row>
     <row r="353">
@@ -3251,7 +3251,7 @@
         <v>351</v>
       </c>
       <c r="B353" t="n">
-        <v>28.36811065673828</v>
+        <v>30.46028900146484</v>
       </c>
     </row>
     <row r="354">
@@ -3259,7 +3259,7 @@
         <v>352</v>
       </c>
       <c r="B354" t="n">
-        <v>28.2815113067627</v>
+        <v>30.45774078369141</v>
       </c>
     </row>
     <row r="355">
@@ -3267,7 +3267,7 @@
         <v>353</v>
       </c>
       <c r="B355" t="n">
-        <v>28.3055591583252</v>
+        <v>30.45569610595703</v>
       </c>
     </row>
     <row r="356">
@@ -3275,7 +3275,7 @@
         <v>354</v>
       </c>
       <c r="B356" t="n">
-        <v>28.43940544128418</v>
+        <v>30.45639419555664</v>
       </c>
     </row>
     <row r="357">
@@ -3283,7 +3283,7 @@
         <v>355</v>
       </c>
       <c r="B357" t="n">
-        <v>28.47974967956543</v>
+        <v>30.45957946777344</v>
       </c>
     </row>
     <row r="358">
@@ -3291,7 +3291,7 @@
         <v>356</v>
       </c>
       <c r="B358" t="n">
-        <v>28.47477912902832</v>
+        <v>30.46245193481445</v>
       </c>
     </row>
     <row r="359">
@@ -3299,7 +3299,7 @@
         <v>357</v>
       </c>
       <c r="B359" t="n">
-        <v>28.47035598754883</v>
+        <v>30.46319770812988</v>
       </c>
     </row>
     <row r="360">
@@ -3307,7 +3307,7 @@
         <v>358</v>
       </c>
       <c r="B360" t="n">
-        <v>28.49332046508789</v>
+        <v>30.46647453308105</v>
       </c>
     </row>
     <row r="361">
@@ -3315,7 +3315,7 @@
         <v>359</v>
       </c>
       <c r="B361" t="n">
-        <v>28.6990966796875</v>
+        <v>30.4635009765625</v>
       </c>
     </row>
     <row r="362">
@@ -3323,7 +3323,7 @@
         <v>360</v>
       </c>
       <c r="B362" t="n">
-        <v>28.58005905151367</v>
+        <v>30.50271224975586</v>
       </c>
     </row>
     <row r="363">
@@ -3331,7 +3331,7 @@
         <v>361</v>
       </c>
       <c r="B363" t="n">
-        <v>28.64844131469727</v>
+        <v>30.51723098754883</v>
       </c>
     </row>
     <row r="364">
@@ -3339,7 +3339,7 @@
         <v>362</v>
       </c>
       <c r="B364" t="n">
-        <v>28.3808536529541</v>
+        <v>30.51758193969727</v>
       </c>
     </row>
     <row r="365">
@@ -3347,7 +3347,7 @@
         <v>363</v>
       </c>
       <c r="B365" t="n">
-        <v>28.20079040527344</v>
+        <v>30.48722457885742</v>
       </c>
     </row>
     <row r="366">
@@ -3355,7 +3355,7 @@
         <v>364</v>
       </c>
       <c r="B366" t="n">
-        <v>28.18913650512695</v>
+        <v>30.48288726806641</v>
       </c>
     </row>
     <row r="367">
@@ -3363,7 +3363,7 @@
         <v>365</v>
       </c>
       <c r="B367" t="n">
-        <v>28.1396656036377</v>
+        <v>30.47560501098633</v>
       </c>
     </row>
     <row r="368">
@@ -3371,7 +3371,7 @@
         <v>366</v>
       </c>
       <c r="B368" t="n">
-        <v>28.21409225463867</v>
+        <v>30.50201797485352</v>
       </c>
     </row>
     <row r="369">
@@ -3379,7 +3379,7 @@
         <v>367</v>
       </c>
       <c r="B369" t="n">
-        <v>28.09102630615234</v>
+        <v>30.50504684448242</v>
       </c>
     </row>
     <row r="370">
@@ -3387,7 +3387,7 @@
         <v>368</v>
       </c>
       <c r="B370" t="n">
-        <v>27.88145446777344</v>
+        <v>30.49808502197266</v>
       </c>
     </row>
     <row r="371">
@@ -3395,7 +3395,7 @@
         <v>369</v>
       </c>
       <c r="B371" t="n">
-        <v>27.89525604248047</v>
+        <v>30.537353515625</v>
       </c>
     </row>
     <row r="372">
@@ -3403,7 +3403,7 @@
         <v>370</v>
       </c>
       <c r="B372" t="n">
-        <v>27.86581802368164</v>
+        <v>30.52213096618652</v>
       </c>
     </row>
     <row r="373">
@@ -3411,7 +3411,7 @@
         <v>371</v>
       </c>
       <c r="B373" t="n">
-        <v>27.58193969726562</v>
+        <v>30.55707168579102</v>
       </c>
     </row>
     <row r="374">
@@ -3419,7 +3419,7 @@
         <v>372</v>
       </c>
       <c r="B374" t="n">
-        <v>27.63134765625</v>
+        <v>30.57456016540527</v>
       </c>
     </row>
     <row r="375">
@@ -3427,7 +3427,7 @@
         <v>373</v>
       </c>
       <c r="B375" t="n">
-        <v>27.37167358398438</v>
+        <v>30.54825973510742</v>
       </c>
     </row>
     <row r="376">
@@ -3435,7 +3435,7 @@
         <v>374</v>
       </c>
       <c r="B376" t="n">
-        <v>27.47225570678711</v>
+        <v>30.5672664642334</v>
       </c>
     </row>
     <row r="377">
@@ -3443,7 +3443,7 @@
         <v>375</v>
       </c>
       <c r="B377" t="n">
-        <v>27.39751052856445</v>
+        <v>30.58523559570312</v>
       </c>
     </row>
     <row r="378">
@@ -3451,7 +3451,7 @@
         <v>376</v>
       </c>
       <c r="B378" t="n">
-        <v>27.44008636474609</v>
+        <v>30.56628608703613</v>
       </c>
     </row>
     <row r="379">
@@ -3459,7 +3459,7 @@
         <v>377</v>
       </c>
       <c r="B379" t="n">
-        <v>27.49541473388672</v>
+        <v>30.56262969970703</v>
       </c>
     </row>
     <row r="380">
@@ -3467,7 +3467,7 @@
         <v>378</v>
       </c>
       <c r="B380" t="n">
-        <v>27.27287483215332</v>
+        <v>30.56840515136719</v>
       </c>
     </row>
     <row r="381">
@@ -3475,7 +3475,7 @@
         <v>379</v>
       </c>
       <c r="B381" t="n">
-        <v>27.35924530029297</v>
+        <v>30.55839157104492</v>
       </c>
     </row>
     <row r="382">
@@ -3483,7 +3483,7 @@
         <v>380</v>
       </c>
       <c r="B382" t="n">
-        <v>27.27735900878906</v>
+        <v>30.57753753662109</v>
       </c>
     </row>
     <row r="383">
@@ -3491,7 +3491,7 @@
         <v>381</v>
       </c>
       <c r="B383" t="n">
-        <v>27.40785789489746</v>
+        <v>30.63239288330078</v>
       </c>
     </row>
     <row r="384">
@@ -3499,7 +3499,7 @@
         <v>382</v>
       </c>
       <c r="B384" t="n">
-        <v>27.3414306640625</v>
+        <v>30.62543106079102</v>
       </c>
     </row>
     <row r="385">
@@ -3507,7 +3507,7 @@
         <v>383</v>
       </c>
       <c r="B385" t="n">
-        <v>27.10245895385742</v>
+        <v>30.65374755859375</v>
       </c>
     </row>
     <row r="386">
@@ -3515,7 +3515,7 @@
         <v>384</v>
       </c>
       <c r="B386" t="n">
-        <v>26.86963081359863</v>
+        <v>30.70275497436523</v>
       </c>
     </row>
     <row r="387">
@@ -3523,7 +3523,7 @@
         <v>385</v>
       </c>
       <c r="B387" t="n">
-        <v>26.87895774841309</v>
+        <v>30.66118431091309</v>
       </c>
     </row>
     <row r="388">
@@ -3531,7 +3531,7 @@
         <v>386</v>
       </c>
       <c r="B388" t="n">
-        <v>26.94759559631348</v>
+        <v>30.65842437744141</v>
       </c>
     </row>
     <row r="389">
@@ -3539,7 +3539,7 @@
         <v>387</v>
       </c>
       <c r="B389" t="n">
-        <v>26.77293395996094</v>
+        <v>30.64432525634766</v>
       </c>
     </row>
     <row r="390">
@@ -3547,7 +3547,7 @@
         <v>388</v>
       </c>
       <c r="B390" t="n">
-        <v>26.88470077514648</v>
+        <v>30.62964057922363</v>
       </c>
     </row>
     <row r="391">
@@ -3555,7 +3555,7 @@
         <v>389</v>
       </c>
       <c r="B391" t="n">
-        <v>26.76132965087891</v>
+        <v>30.63294982910156</v>
       </c>
     </row>
     <row r="392">
@@ -3563,7 +3563,7 @@
         <v>390</v>
       </c>
       <c r="B392" t="n">
-        <v>26.79189491271973</v>
+        <v>30.6537971496582</v>
       </c>
     </row>
     <row r="393">
@@ -3571,7 +3571,7 @@
         <v>391</v>
       </c>
       <c r="B393" t="n">
-        <v>26.59012603759766</v>
+        <v>30.643798828125</v>
       </c>
     </row>
     <row r="394">
@@ -3579,7 +3579,7 @@
         <v>392</v>
       </c>
       <c r="B394" t="n">
-        <v>26.52219772338867</v>
+        <v>30.65868377685547</v>
       </c>
     </row>
     <row r="395">
@@ -3587,7 +3587,7 @@
         <v>393</v>
       </c>
       <c r="B395" t="n">
-        <v>26.94721984863281</v>
+        <v>30.66427230834961</v>
       </c>
     </row>
     <row r="396">
@@ -3595,7 +3595,7 @@
         <v>394</v>
       </c>
       <c r="B396" t="n">
-        <v>27.20983695983887</v>
+        <v>30.67323684692383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>